<commit_message>
fixed some wrong text
</commit_message>
<xml_diff>
--- a/data/ordini.xlsx
+++ b/data/ordini.xlsx
@@ -5,22 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlasala\Work Folders\Desktop\progetti\scadenziario\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlasala\Work Folders\Desktop\progetti\scadenziario_codex\order_helper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313CB6A4-3D37-4191-AD16-8CE9460A4E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4ADD6AE-1A31-4E9A-A1A0-25E37FD37725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="8040" windowWidth="28590" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9495" yWindow="2685" windowWidth="28590" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ordini" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ordini!$A$1:$J$37</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="100">
   <si>
     <t>Codice</t>
   </si>
@@ -71,6 +74,255 @@
   </si>
   <si>
     <t>26/08/2025</t>
+  </si>
+  <si>
+    <t>SL2524  -  MOTORE INTERNO BRUSHLESS SL27/32M (CON RP22SS4) REV. 2 - Montaggio</t>
+  </si>
+  <si>
+    <t>2024-OF-0000808</t>
+  </si>
+  <si>
+    <t>SL1084B160-L</t>
+  </si>
+  <si>
+    <t>SL1084B160  -  MODULO SOLARE B160 REV. 4 - Montaggio</t>
+  </si>
+  <si>
+    <t>2024-OF-0003097</t>
+  </si>
+  <si>
+    <t>2024-OF-0003098</t>
+  </si>
+  <si>
+    <t>SL3192-L</t>
+  </si>
+  <si>
+    <t>SL3192  -  TELECOMANDO RADIO - Montaggio</t>
+  </si>
+  <si>
+    <t>2024-OF-0003715</t>
+  </si>
+  <si>
+    <t>SL3199-L</t>
+  </si>
+  <si>
+    <t>SL3199  -  MOTORIDUTTORE SL27/29/32 MB PELLINI - Montaggio</t>
+  </si>
+  <si>
+    <t>2024-OF-0003902</t>
+  </si>
+  <si>
+    <t>2024-OF-0004048</t>
+  </si>
+  <si>
+    <t>2024-OF-0004051</t>
+  </si>
+  <si>
+    <t>SL2395-L</t>
+  </si>
+  <si>
+    <t>SL2395  -  MOTORE INTERNO SL20/22 W  REV.3 - Montaggio</t>
+  </si>
+  <si>
+    <t>2024-OF-0004431</t>
+  </si>
+  <si>
+    <t>SL2775S102-L</t>
+  </si>
+  <si>
+    <t>SL2775S102  -  SUPPORTO MODULO BATTERIA BIANCO REV. 1 - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0000302</t>
+  </si>
+  <si>
+    <t>2025-OF-0000303</t>
+  </si>
+  <si>
+    <t>SL2775S157-L</t>
+  </si>
+  <si>
+    <t>SL2775S157  -  SUPPORTO MODULO BATTERIA ARGENTO - REV. 1 - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0000333</t>
+  </si>
+  <si>
+    <t>SL2776S157-L</t>
+  </si>
+  <si>
+    <t>SL2776S157  -  MODULO BATTERIA ARGENTO REV. 3 - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0000342</t>
+  </si>
+  <si>
+    <t>2025-OF-0000497</t>
+  </si>
+  <si>
+    <t>SLAV</t>
+  </si>
+  <si>
+    <t>BB0000003 - Recupero nel processo produttivo tramite ricarica in reparto elettronico</t>
+  </si>
+  <si>
+    <t>2025-OF-0000753</t>
+  </si>
+  <si>
+    <t>SL3107-L</t>
+  </si>
+  <si>
+    <t>SL3107  -  CENTRALINA MOTORE 24V - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0000815</t>
+  </si>
+  <si>
+    <t>SL3000B-L</t>
+  </si>
+  <si>
+    <t>SL3000B  -  MODULO BASE HUB CONTROLLO TENDE - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0000849</t>
+  </si>
+  <si>
+    <t>SL2921B160-L</t>
+  </si>
+  <si>
+    <t>SL2921B160  -  GRUPPO MOTORE 24V WAVE B160 REV.1 - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0001091</t>
+  </si>
+  <si>
+    <t>SL2190-L</t>
+  </si>
+  <si>
+    <t>SL2190  -  MOTORE ESTERNO rev.5 (*) - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0001155</t>
+  </si>
+  <si>
+    <t>SL2497-L</t>
+  </si>
+  <si>
+    <t>SL2497  -  MOTORE INTERNO SL27/32 M PER ALBERO ESAGONALE 5MM REV.3 - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0001184</t>
+  </si>
+  <si>
+    <t>SL3251-L</t>
+  </si>
+  <si>
+    <t>SL3251  -  MOTORE INTERNO SL20/22 Wÿ - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0001215</t>
+  </si>
+  <si>
+    <t>SL3252-L</t>
+  </si>
+  <si>
+    <t>SL3252  -  MOTORE INTERNO SL27/29/32 W - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0001224</t>
+  </si>
+  <si>
+    <t>2025-OF-0001329</t>
+  </si>
+  <si>
+    <t>SL2420-L</t>
+  </si>
+  <si>
+    <t>SL2420  -  TEST KIT 3 VOLT S157 - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0001978</t>
+  </si>
+  <si>
+    <t>2025-OF-0002036</t>
+  </si>
+  <si>
+    <t>SL1032S000-L</t>
+  </si>
+  <si>
+    <t>SL1032S000  -  COMANDO ESTERNO AD ASTA TRASPARENTE (*) - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0002049</t>
+  </si>
+  <si>
+    <t>2025-OF-0002080</t>
+  </si>
+  <si>
+    <t>SL2534-L</t>
+  </si>
+  <si>
+    <t>SL2534  -  TEST KIT PER TENDE 24V REV. 1 - Produzione</t>
+  </si>
+  <si>
+    <t>2025-OF-0002131</t>
+  </si>
+  <si>
+    <t>SL3071-L</t>
+  </si>
+  <si>
+    <t>SL3071  -  MOTORE INTERNO SL27/29/32 MB PELLINI - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0002165</t>
+  </si>
+  <si>
+    <t>2025-OF-0002166</t>
+  </si>
+  <si>
+    <t>SL3157S102-L</t>
+  </si>
+  <si>
+    <t>SL3157S102  -  COMANDO ESTERNO A LEVA S102 - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0002188</t>
+  </si>
+  <si>
+    <t>SL3157S155-L</t>
+  </si>
+  <si>
+    <t>SL3157S155  -  COMANDO ESTERNO A LEVA S155 - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0002189</t>
+  </si>
+  <si>
+    <t>SL3160S102-L</t>
+  </si>
+  <si>
+    <t>SL3160S102  -  COMANDO CON CHIAVE S102 - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0002190</t>
+  </si>
+  <si>
+    <t>SL3160S155-L</t>
+  </si>
+  <si>
+    <t>SL3160S155  -  COMANDO CON CHIAVE S155 - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0002191</t>
+  </si>
+  <si>
+    <t>SL2776S102-L</t>
+  </si>
+  <si>
+    <t>SL2776S102  -  MODULO BATTERIA BIANCO  REV.3 - Montaggio</t>
+  </si>
+  <si>
+    <t>2025-OF-0002269</t>
   </si>
 </sst>
 </file>
@@ -126,11 +378,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -433,13 +687,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:J16"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -493,7 +756,7 @@
         <v>0.08</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>9432</v>
@@ -537,7 +800,1012 @@
         <v>16</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>500</v>
+      </c>
+      <c r="D4">
+        <v>500</v>
+      </c>
+      <c r="E4">
+        <v>600</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="2">
+        <v>45364</v>
+      </c>
+      <c r="J4" s="2">
+        <v>45853</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>500</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+      <c r="E5">
+        <v>640</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="2">
+        <v>45551</v>
+      </c>
+      <c r="J5" s="2">
+        <v>45823</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>500</v>
+      </c>
+      <c r="D6">
+        <v>500</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1600</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="2">
+        <v>45551</v>
+      </c>
+      <c r="J6" s="2">
+        <v>45853</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>400</v>
+      </c>
+      <c r="D7">
+        <v>400</v>
+      </c>
+      <c r="E7">
+        <v>560</v>
+      </c>
+      <c r="F7">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="2">
+        <v>45588</v>
+      </c>
+      <c r="J7" s="2">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="2">
+        <v>45604</v>
+      </c>
+      <c r="J8" s="2">
+        <v>45807</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>500</v>
+      </c>
+      <c r="D9">
+        <v>500</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="2">
+        <v>45615</v>
+      </c>
+      <c r="J9" s="2">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10">
+        <v>500</v>
+      </c>
+      <c r="D10">
+        <v>500</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="2">
+        <v>45615</v>
+      </c>
+      <c r="J10" s="2">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1479</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1159</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1622.6</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="2">
+        <v>45642</v>
+      </c>
+      <c r="J11" s="2">
+        <v>45838</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>500</v>
+      </c>
+      <c r="D12">
+        <v>250</v>
+      </c>
+      <c r="E12">
+        <v>320</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="2">
+        <v>45684</v>
+      </c>
+      <c r="J12" s="2">
+        <v>45842</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13">
+        <v>500</v>
+      </c>
+      <c r="D13">
+        <v>500</v>
+      </c>
+      <c r="E13">
+        <v>640</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="2">
+        <v>45684</v>
+      </c>
+      <c r="J13" s="2">
+        <v>45849</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14">
+        <v>500</v>
+      </c>
+      <c r="D14">
+        <v>500</v>
+      </c>
+      <c r="E14">
+        <v>640</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="2">
+        <v>45684</v>
+      </c>
+      <c r="J14" s="2">
+        <v>45842</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15">
+        <v>300</v>
+      </c>
+      <c r="D15">
+        <v>300</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1320</v>
+      </c>
+      <c r="F15">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="2">
+        <v>45684</v>
+      </c>
+      <c r="J15" s="2">
+        <v>45853</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>400</v>
+      </c>
+      <c r="D16">
+        <v>400</v>
+      </c>
+      <c r="E16">
+        <v>560</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="2">
+        <v>45699</v>
+      </c>
+      <c r="J16" s="2">
+        <v>45849</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17">
+        <v>257</v>
+      </c>
+      <c r="D17">
+        <v>257</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" s="2">
+        <v>45720</v>
+      </c>
+      <c r="J17" s="2">
+        <v>45781</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18">
+        <v>800</v>
+      </c>
+      <c r="D18">
+        <v>800</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1600</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" s="2">
+        <v>45723</v>
+      </c>
+      <c r="J18" s="2">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19">
+        <v>45</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="2">
+        <v>45727</v>
+      </c>
+      <c r="J19" s="2">
+        <v>45747</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20">
+        <v>500</v>
+      </c>
+      <c r="D20">
+        <v>500</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1200</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" s="2">
+        <v>45744</v>
+      </c>
+      <c r="J20" s="2">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21">
+        <v>330</v>
+      </c>
+      <c r="D21">
+        <v>330</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="2">
+        <v>45754</v>
+      </c>
+      <c r="J21" s="2">
+        <v>45838</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22">
+        <v>483</v>
+      </c>
+      <c r="D22">
+        <v>483</v>
+      </c>
+      <c r="E22">
+        <v>483</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" s="2">
+        <v>45755</v>
+      </c>
+      <c r="J22" s="2">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1500</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1500</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>65</v>
+      </c>
+      <c r="I23" s="2">
+        <v>45756</v>
+      </c>
+      <c r="J23" s="2">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24">
+        <v>139</v>
+      </c>
+      <c r="D24">
+        <v>139</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" s="2">
+        <v>45756</v>
+      </c>
+      <c r="J24" s="2">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25">
+        <v>200</v>
+      </c>
+      <c r="D25">
+        <v>200</v>
+      </c>
+      <c r="E25">
+        <v>256</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>69</v>
+      </c>
+      <c r="I25" s="2">
+        <v>45763</v>
+      </c>
+      <c r="J25" s="2">
+        <v>45842</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>19</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>72</v>
+      </c>
+      <c r="I26" s="2">
+        <v>45825</v>
+      </c>
+      <c r="J26" s="2">
+        <v>45846</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>500</v>
+      </c>
+      <c r="D27">
+        <v>500</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1600</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" s="2">
+        <v>45827</v>
+      </c>
+      <c r="J27" s="2">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28">
+        <v>100</v>
+      </c>
+      <c r="D28">
+        <v>100</v>
+      </c>
+      <c r="E28">
+        <v>80</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>76</v>
+      </c>
+      <c r="I28" s="2">
+        <v>45828</v>
+      </c>
+      <c r="J28" s="2">
+        <v>45863</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29">
+        <v>300</v>
+      </c>
+      <c r="D29">
+        <v>300</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
+        <v>77</v>
+      </c>
+      <c r="I29" s="2">
+        <v>45832</v>
+      </c>
+      <c r="J29" s="2">
+        <v>45863</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30">
+        <v>30</v>
+      </c>
+      <c r="D30">
+        <v>20</v>
+      </c>
+      <c r="E30">
+        <v>120</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>80</v>
+      </c>
+      <c r="I30" s="2">
+        <v>45838</v>
+      </c>
+      <c r="J30" s="2">
+        <v>45838</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31">
+        <v>500</v>
+      </c>
+      <c r="D31">
+        <v>450</v>
+      </c>
+      <c r="E31">
+        <v>540</v>
+      </c>
+      <c r="F31">
+        <v>0.1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>83</v>
+      </c>
+      <c r="I31" s="2">
+        <v>45840</v>
+      </c>
+      <c r="J31" s="2">
+        <v>45863</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32">
+        <v>500</v>
+      </c>
+      <c r="D32">
+        <v>500</v>
+      </c>
+      <c r="E32">
+        <v>600</v>
+      </c>
+      <c r="F32">
+        <v>0.1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>84</v>
+      </c>
+      <c r="I32" s="2">
+        <v>45840</v>
+      </c>
+      <c r="J32" s="2">
+        <v>45863</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33">
+        <v>100</v>
+      </c>
+      <c r="D33">
+        <v>100</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>87</v>
+      </c>
+      <c r="I33" s="2">
+        <v>45841</v>
+      </c>
+      <c r="J33" s="2">
+        <v>45853</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34">
+        <v>100</v>
+      </c>
+      <c r="D34">
+        <v>100</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>90</v>
+      </c>
+      <c r="I34" s="2">
+        <v>45841</v>
+      </c>
+      <c r="J34" s="2">
+        <v>45853</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35">
+        <v>100</v>
+      </c>
+      <c r="D35">
+        <v>100</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>93</v>
+      </c>
+      <c r="I35" s="2">
+        <v>45841</v>
+      </c>
+      <c r="J35" s="2">
+        <v>45853</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36">
+        <v>100</v>
+      </c>
+      <c r="D36">
+        <v>100</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>96</v>
+      </c>
+      <c r="I36" s="2">
+        <v>45841</v>
+      </c>
+      <c r="J36" s="2">
+        <v>45853</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37">
+        <v>100</v>
+      </c>
+      <c r="D37">
+        <v>100</v>
+      </c>
+      <c r="E37">
+        <v>440</v>
+      </c>
+      <c r="F37">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>99</v>
+      </c>
+      <c r="I37" s="2">
+        <v>45847</v>
+      </c>
+      <c r="J37" s="2">
+        <v>45869</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:J37" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>